<commit_message>
Added Import MD Tool without sync for testing purposes
</commit_message>
<xml_diff>
--- a/Data Standards+Metadata Checklist.xlsx
+++ b/Data Standards+Metadata Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHallock\Desktop\ArcGIS Scripts\Data Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A14516-20C3-45D6-8693-7CF9D36B61B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2C9AF8-0EEF-4B7C-975F-4B5A0CF0048A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
     <sheet name="Functions" sheetId="3" r:id="rId2"/>
     <sheet name="Debug Functions" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="81">
   <si>
     <t>Add Data Standards(Fields and MD)</t>
   </si>
@@ -218,10 +219,58 @@
     <t>Checks Field MD</t>
   </si>
   <si>
-    <t>Checks Overal MD</t>
-  </si>
-  <si>
     <t>Checks Domains of Field MD</t>
+  </si>
+  <si>
+    <t>Add Missing MD Fields</t>
+  </si>
+  <si>
+    <t>Remove/Rename extra MD Fields</t>
+  </si>
+  <si>
+    <t>Thoughts:</t>
+  </si>
+  <si>
+    <t>Potential order</t>
+  </si>
+  <si>
+    <t>Check quality first always in case of md fields to be renamed?</t>
+  </si>
+  <si>
+    <t>Then maybe in fix fields have a rename/reassign option?</t>
+  </si>
+  <si>
+    <t>only removes, no renames</t>
+  </si>
+  <si>
+    <t>only renames core, others get removed</t>
+  </si>
+  <si>
+    <t>* Tell if source/description is missing</t>
+  </si>
+  <si>
+    <t>Fix order but don't delete extra fields</t>
+  </si>
+  <si>
+    <t>Remove Dupes of core</t>
+  </si>
+  <si>
+    <t>Checkbox for deleting Fields that no longer exist + list to rename them</t>
+  </si>
+  <si>
+    <t>Checks Overall MD</t>
+  </si>
+  <si>
+    <t>* Checks for/Replaces Placeholders</t>
+  </si>
+  <si>
+    <t>Checks for placeholders</t>
+  </si>
+  <si>
+    <t>Add Placeholders to MD values that should be filled</t>
+  </si>
+  <si>
+    <t>y (At end)</t>
   </si>
 </sst>
 </file>
@@ -482,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -504,6 +553,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -516,11 +568,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <border>
         <left style="thin">
@@ -566,22 +621,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -905,17 +944,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="10" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
@@ -929,26 +968,26 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="18"/>
+      <c r="K1" s="19"/>
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,19 +1175,19 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>12</v>
@@ -1247,51 +1286,51 @@
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>12</v>
@@ -1302,7 +1341,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>10</v>
@@ -1323,7 +1362,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>10</v>
@@ -1337,7 +1376,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>10</v>
@@ -1358,7 +1397,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>10</v>
@@ -1372,28 +1411,28 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>10</v>
@@ -1405,33 +1444,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>12</v>
@@ -1440,33 +1479,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>12</v>
+        <v>65</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>12</v>
@@ -1475,24 +1514,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>12</v>
@@ -1504,77 +1543,77 @@
         <v>12</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="s">
-        <v>12</v>
+      <c r="C18" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>12</v>
@@ -1582,36 +1621,211 @@
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="12" t="s">
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1624,18 +1838,18 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K1048576">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1646,11 +1860,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D037D56-654E-4299-841C-27C58773C05D}">
-  <dimension ref="A1:AR29"/>
+  <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,72 +1916,72 @@
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19" t="s">
+      <c r="M1" s="19"/>
+      <c r="N1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19" t="s">
+      <c r="O1" s="19"/>
+      <c r="P1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="19" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="19" t="s">
+      <c r="S1" s="19"/>
+      <c r="T1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="18"/>
-      <c r="V1" s="19" t="s">
+      <c r="U1" s="19"/>
+      <c r="V1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="19" t="s">
+      <c r="W1" s="19"/>
+      <c r="X1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="19"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="20"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="21"/>
+      <c r="AQ1" s="21"/>
       <c r="AR1" s="16"/>
     </row>
     <row r="2" spans="1:44" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3316,9 +3530,9 @@
       <c r="AO20" s="12"/>
       <c r="AQ20" s="12"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>12</v>
@@ -3357,7 +3571,7 @@
         <v>12</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="O21" s="12" t="s">
         <v>12</v>
@@ -3369,16 +3583,16 @@
         <v>12</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="S21" s="12" t="s">
         <v>12</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U21" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>12</v>
@@ -3404,7 +3618,7 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>12</v>
@@ -3490,7 +3704,7 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>12</v>
@@ -3547,13 +3761,13 @@
         <v>12</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="V23" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W23" s="12" t="s">
         <v>12</v>
@@ -3576,7 +3790,7 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>12</v>
@@ -3593,62 +3807,62 @@
       <c r="F24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S24" t="s">
+      <c r="S24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="U24" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="V24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Y24" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA24" s="12"/>
       <c r="AC24" s="12"/>
@@ -3661,37 +3875,275 @@
       <c r="AQ24" s="12"/>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="G25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="U25" s="12"/>
-      <c r="W25" s="12"/>
+      <c r="A25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="W25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="X25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y25" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AE25" s="12"/>
+      <c r="AG25" s="12"/>
+      <c r="AI25" s="12"/>
+      <c r="AK25" s="12"/>
+      <c r="AM25" s="12"/>
+      <c r="AO25" s="12"/>
+      <c r="AQ25" s="12"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="G26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="U26" s="12"/>
-      <c r="W26" s="12"/>
-    </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="G29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="W29" s="12"/>
+      <c r="A26" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>12</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S26" t="s">
+        <v>12</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U26" t="s">
+        <v>12</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W26" t="s">
+        <v>12</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AQ26" s="12"/>
+    </row>
+    <row r="27" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" t="s">
+        <v>12</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>12</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S27" t="s">
+        <v>12</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U27" t="s">
+        <v>12</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W27" t="s">
+        <v>12</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y27" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="G28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="W28" s="12"/>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="G31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="W31" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -3729,7 +4181,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AA1048576 AC3:AC1048576 AE3:AE1048576 AG3:AG1048576 AI3:AI1048576 AK3:AK1048576 AM3:AM1048576 AO3:AO1048576 AQ3:AQ1048576 C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576 M3:M1048576 O3:O1048576 Q3:Q1048576 S3:S1048576 U3:U1048576 W3:W1048576 Y3:Y1048576">
-    <cfRule type="expression" dxfId="4" priority="61">
+    <cfRule type="expression" dxfId="0" priority="61">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3771,4 +4223,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009F32E3-3FEE-430F-A708-D6066633E4B1}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed JustAddMetadata and Reordered Tools
</commit_message>
<xml_diff>
--- a/Data Standards+Metadata Checklist.xlsx
+++ b/Data Standards+Metadata Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHallock\Desktop\ArcGIS Scripts\Data Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9773625E-FD5A-42BF-93ED-039CC3AE4A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8714DD36-E81F-45CE-BDB0-7A4BF0E5A254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="97">
   <si>
     <t>Add Data Standards(Fields and MD)</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Import Unsynced Metadata</t>
+  </si>
+  <si>
+    <t>Check for Placeholder Values</t>
   </si>
 </sst>
 </file>
@@ -345,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -557,11 +560,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -591,23 +603,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -637,22 +655,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -791,36 +793,6 @@
           <color rgb="FF9C0006"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1098,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,27 +1095,27 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="20"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="20"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="20"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="20"/>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>94</v>
       </c>
       <c r="M1" s="20"/>
@@ -1325,10 +1297,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>18</v>
@@ -1820,7 +1792,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>76</v>
@@ -1861,7 +1833,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>10</v>
@@ -1895,14 +1867,14 @@
       <c r="B21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="23" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>10</v>
@@ -2257,44 +2229,85 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M30" s="11" t="s">
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M31" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2308,45 +2321,45 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K1048576">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576">
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:M29">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+  <conditionalFormatting sqref="L3:M30">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M30">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="M3:M31">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>L3&lt;&gt;M3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L30:M30">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="L31:M31">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2359,9 +2372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D037D56-654E-4299-841C-27C58773C05D}">
   <dimension ref="A1:AR34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L3" sqref="L3:AC11"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,75 +2426,75 @@
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="20"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G1" s="20"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>82</v>
       </c>
       <c r="I1" s="20"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="20"/>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>31</v>
       </c>
       <c r="M1" s="20"/>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>33</v>
       </c>
       <c r="O1" s="20"/>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="19" t="s">
         <v>32</v>
       </c>
       <c r="Q1" s="20"/>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="19" t="s">
         <v>34</v>
       </c>
       <c r="S1" s="20"/>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="19" t="s">
         <v>39</v>
       </c>
       <c r="U1" s="20"/>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="19" t="s">
         <v>38</v>
       </c>
       <c r="W1" s="20"/>
-      <c r="X1" s="21" t="s">
+      <c r="X1" s="19" t="s">
         <v>35</v>
       </c>
       <c r="Y1" s="20"/>
-      <c r="Z1" s="21" t="s">
+      <c r="Z1" s="19" t="s">
         <v>36</v>
       </c>
       <c r="AA1" s="20"/>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="19" t="s">
         <v>37</v>
       </c>
       <c r="AC1" s="20"/>
-      <c r="AD1" s="21" t="s">
+      <c r="AD1" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AE1" s="20"/>
-      <c r="AF1" s="21"/>
+      <c r="AF1" s="19"/>
       <c r="AG1" s="20"/>
-      <c r="AH1" s="21"/>
+      <c r="AH1" s="19"/>
       <c r="AI1" s="20"/>
-      <c r="AJ1" s="21"/>
+      <c r="AJ1" s="19"/>
       <c r="AK1" s="20"/>
-      <c r="AL1" s="21"/>
+      <c r="AL1" s="19"/>
       <c r="AM1" s="20"/>
-      <c r="AN1" s="21"/>
+      <c r="AN1" s="19"/>
       <c r="AO1" s="20"/>
       <c r="AP1" s="22"/>
       <c r="AQ1" s="22"/>
@@ -5817,6 +5830,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AP1:AQ1"/>
@@ -5833,25 +5851,20 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:AQ1048576">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576 M3:M1048576 O3:O1048576 Q3:Q1048576 S3:S1048576 U3:U1048576 W3:W1048576 Y3:Y1048576 AA3:AA1048576 AC3:AC1048576 AE3:AE1048576 AG3:AG1048576 AI3:AI1048576 AK3:AK1048576 AM3:AM1048576 AO3:AO1048576 AQ3:AQ1048576">
-    <cfRule type="expression" dxfId="11" priority="61">
+    <cfRule type="expression" dxfId="6" priority="61">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Interface for Fix Fields Metadata Tool
</commit_message>
<xml_diff>
--- a/Data Standards+Metadata Checklist.xlsx
+++ b/Data Standards+Metadata Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHallock\Desktop\ArcGIS Scripts\Data Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8714DD36-E81F-45CE-BDB0-7A4BF0E5A254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58A9E6-B502-40EE-B5F6-9973FC262B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="99">
   <si>
     <t>Add Data Standards(Fields and MD)</t>
   </si>
@@ -319,6 +320,12 @@
   </si>
   <si>
     <t>Check for Placeholder Values</t>
+  </si>
+  <si>
+    <t>FixFieldMDDescsEtc</t>
+  </si>
+  <si>
+    <t>Adds Placeholders when needed</t>
   </si>
 </sst>
 </file>
@@ -348,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -569,11 +576,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -603,6 +651,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,46 +674,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="12">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -777,22 +816,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1070,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,37 +1113,38 @@
     <col min="10" max="10" width="15.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="13.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="20"/>
-    </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="27"/>
+      <c r="N1" s="21"/>
+    </row>
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>5</v>
@@ -1155,11 +1179,12 @@
       <c r="L2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
@@ -1187,9 +1212,9 @@
       <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="11"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>77</v>
       </c>
@@ -1215,9 +1240,9 @@
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>85</v>
       </c>
@@ -1243,9 +1268,9 @@
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="24"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
@@ -1282,11 +1307,11 @@
       <c r="L6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M6" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>78</v>
       </c>
@@ -1303,10 +1328,10 @@
         <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>18</v>
@@ -1323,11 +1348,11 @@
       <c r="L7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -1364,11 +1389,11 @@
       <c r="L8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1405,11 +1430,11 @@
       <c r="L9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M9" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1446,11 +1471,11 @@
       <c r="L10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="M10" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>88</v>
       </c>
@@ -1487,11 +1512,11 @@
       <c r="L11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M11" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>89</v>
       </c>
@@ -1528,11 +1553,11 @@
       <c r="L12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M12" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -1569,11 +1594,11 @@
       <c r="L13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -1593,7 +1618,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>12</v>
@@ -1610,11 +1635,11 @@
       <c r="L14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -1651,11 +1676,11 @@
       <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M15" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>75</v>
       </c>
@@ -1675,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>10</v>
@@ -1692,7 +1717,7 @@
       <c r="L16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1733,7 +1758,7 @@
       <c r="L17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1774,7 +1799,7 @@
       <c r="L18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1815,7 +1840,7 @@
       <c r="L19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1856,7 +1881,7 @@
       <c r="L20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1867,10 +1892,10 @@
       <c r="B21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="19" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="16" t="s">
@@ -1897,7 +1922,7 @@
       <c r="L21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1938,7 +1963,7 @@
       <c r="L22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="11" t="s">
+      <c r="M22" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1979,7 +2004,7 @@
       <c r="L23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2020,7 +2045,7 @@
       <c r="L24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M24" s="11" t="s">
+      <c r="M24" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2061,7 +2086,7 @@
       <c r="L25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M25" s="11" t="s">
+      <c r="M25" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2102,7 +2127,7 @@
       <c r="L26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M26" s="11" t="s">
+      <c r="M26" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2143,7 +2168,7 @@
       <c r="L27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M27" s="11" t="s">
+      <c r="M27" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2184,7 +2209,7 @@
       <c r="L28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="11" t="s">
+      <c r="M28" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2225,7 +2250,7 @@
       <c r="L29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M29" s="11" t="s">
+      <c r="M29" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2266,7 +2291,7 @@
       <c r="L30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M30" s="11" t="s">
+      <c r="M30" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2307,7 +2332,7 @@
       <c r="L31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="24" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2321,46 +2346,35 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K1048576">
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576">
-    <cfRule type="expression" dxfId="14" priority="11">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:M30">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+  <conditionalFormatting sqref="L3:M31">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M31">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>L3&lt;&gt;M3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L31:M31">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"?"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"n"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2370,11 +2384,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D037D56-654E-4299-841C-27C58773C05D}">
-  <dimension ref="A1:AR34"/>
+  <dimension ref="A1:AR35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,8 +2414,8 @@
     <col min="19" max="19" width="13.28515625" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" style="2" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" customWidth="1"/>
     <col min="24" max="24" width="13.28515625" style="2" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" customWidth="1"/>
     <col min="26" max="26" width="13.28515625" style="2" customWidth="1"/>
@@ -2426,78 +2440,80 @@
   <sheetData>
     <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="19" t="s">
+      <c r="M1" s="27"/>
+      <c r="N1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="19" t="s">
+      <c r="O1" s="27"/>
+      <c r="P1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="19" t="s">
+      <c r="Q1" s="27"/>
+      <c r="R1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="20"/>
-      <c r="T1" s="19" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="27"/>
+      <c r="V1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="20"/>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="19" t="s">
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
       <c r="AR1" s="15"/>
     </row>
     <row r="2" spans="1:44" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2694,13 +2710,13 @@
         <v>10</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>10</v>
@@ -2720,7 +2736,12 @@
       <c r="AE3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG3" s="11"/>
+      <c r="AF3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI3" s="11"/>
       <c r="AK3" s="11"/>
       <c r="AM3" s="11"/>
@@ -2821,7 +2842,12 @@
       <c r="AE4" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG4" s="11"/>
+      <c r="AF4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AM4" s="11"/>
@@ -2922,7 +2948,12 @@
       <c r="AE5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG5" s="11"/>
+      <c r="AF5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG5" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI5" s="11"/>
       <c r="AK5" s="11"/>
       <c r="AM5" s="11"/>
@@ -3023,7 +3054,12 @@
       <c r="AE6" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG6" s="11"/>
+      <c r="AF6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI6" s="11"/>
       <c r="AK6" s="11"/>
       <c r="AM6" s="11"/>
@@ -3124,7 +3160,12 @@
       <c r="AE7" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG7" s="11"/>
+      <c r="AF7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG7" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI7" s="11"/>
       <c r="AK7" s="11"/>
       <c r="AM7" s="11"/>
@@ -3225,7 +3266,12 @@
       <c r="AE8" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG8" s="11"/>
+      <c r="AF8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG8" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI8" s="11"/>
       <c r="AK8" s="11"/>
       <c r="AM8" s="11"/>
@@ -3326,7 +3372,12 @@
       <c r="AE9" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG9" s="11"/>
+      <c r="AF9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG9" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI9" s="11"/>
       <c r="AK9" s="11"/>
       <c r="AM9" s="11"/>
@@ -3427,7 +3478,12 @@
       <c r="AE10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG10" s="11"/>
+      <c r="AF10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG10" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI10" s="11"/>
       <c r="AK10" s="11"/>
       <c r="AM10" s="11"/>
@@ -3528,7 +3584,12 @@
       <c r="AE11" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="AG11" s="11"/>
+      <c r="AF11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG11" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="AI11" s="11"/>
       <c r="AK11" s="11"/>
       <c r="AM11" s="11"/>
@@ -3629,7 +3690,12 @@
       <c r="AE12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG12" s="11"/>
+      <c r="AF12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG12" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI12" s="11"/>
       <c r="AK12" s="11"/>
       <c r="AM12" s="11"/>
@@ -3730,7 +3796,12 @@
       <c r="AE13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG13" s="11"/>
+      <c r="AF13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG13" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI13" s="11"/>
       <c r="AK13" s="11"/>
       <c r="AM13" s="11"/>
@@ -3831,7 +3902,12 @@
       <c r="AE14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG14" s="11"/>
+      <c r="AF14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG14" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI14" s="11"/>
       <c r="AK14" s="11"/>
       <c r="AM14" s="11"/>
@@ -3932,7 +4008,12 @@
       <c r="AE15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG15" s="11"/>
+      <c r="AF15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG15" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI15" s="11"/>
       <c r="AK15" s="11"/>
       <c r="AM15" s="11"/>
@@ -4033,7 +4114,12 @@
       <c r="AE16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG16" s="11"/>
+      <c r="AF16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG16" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI16" s="11"/>
       <c r="AK16" s="11"/>
       <c r="AM16" s="11"/>
@@ -4134,7 +4220,12 @@
       <c r="AE17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG17" s="11"/>
+      <c r="AF17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG17" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI17" s="11"/>
       <c r="AK17" s="11"/>
       <c r="AM17" s="11"/>
@@ -4235,7 +4326,12 @@
       <c r="AE18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG18" s="11"/>
+      <c r="AF18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG18" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI18" s="11"/>
       <c r="AK18" s="11"/>
       <c r="AM18" s="11"/>
@@ -4336,7 +4432,12 @@
       <c r="AE19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG19" s="11"/>
+      <c r="AF19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG19" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI19" s="11"/>
       <c r="AK19" s="11"/>
       <c r="AM19" s="11"/>
@@ -4437,7 +4538,12 @@
       <c r="AE20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG20" s="11"/>
+      <c r="AF20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG20" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI20" s="11"/>
       <c r="AK20" s="11"/>
       <c r="AM20" s="11"/>
@@ -4521,10 +4627,10 @@
         <v>10</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA21" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB21" s="2" t="s">
         <v>12</v>
@@ -4538,7 +4644,12 @@
       <c r="AE21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG21" s="11"/>
+      <c r="AF21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG21" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI21" s="11"/>
       <c r="AK21" s="11"/>
       <c r="AM21" s="11"/>
@@ -4622,10 +4733,10 @@
         <v>10</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA22" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB22" s="2" t="s">
         <v>12</v>
@@ -4639,7 +4750,12 @@
       <c r="AE22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG22" s="11"/>
+      <c r="AF22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG22" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI22" s="11"/>
       <c r="AK22" s="11"/>
       <c r="AM22" s="11"/>
@@ -4708,7 +4824,7 @@
         <v>10</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V23" s="2" t="s">
         <v>10</v>
@@ -4720,14 +4836,14 @@
         <v>10</v>
       </c>
       <c r="Y23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="Z23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA23" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="AB23" s="2" t="s">
         <v>12</v>
       </c>
@@ -4740,7 +4856,12 @@
       <c r="AE23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG23" s="11"/>
+      <c r="AF23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG23" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI23" s="11"/>
       <c r="AK23" s="11"/>
       <c r="AM23" s="11"/>
@@ -4806,10 +4927,10 @@
         <v>12</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>10</v>
@@ -4824,10 +4945,10 @@
         <v>10</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA24" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB24" s="2" t="s">
         <v>12</v>
@@ -4841,7 +4962,12 @@
       <c r="AE24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG24" s="11"/>
+      <c r="AF24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG24" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI24" s="11"/>
       <c r="AK24" s="11"/>
       <c r="AM24" s="11"/>
@@ -4907,10 +5033,10 @@
         <v>12</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>10</v>
@@ -4925,10 +5051,10 @@
         <v>10</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA25" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB25" s="2" t="s">
         <v>12</v>
@@ -4942,7 +5068,12 @@
       <c r="AE25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG25" s="11"/>
+      <c r="AF25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG25" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI25" s="11"/>
       <c r="AK25" s="11"/>
       <c r="AM25" s="11"/>
@@ -5008,16 +5139,16 @@
         <v>12</v>
       </c>
       <c r="T26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="V26" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="W26" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X26" s="2" t="s">
         <v>10</v>
@@ -5026,10 +5157,10 @@
         <v>10</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA26" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB26" s="2" t="s">
         <v>12</v>
@@ -5043,7 +5174,12 @@
       <c r="AE26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG26" s="11"/>
+      <c r="AF26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG26" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI26" s="11"/>
       <c r="AK26" s="11"/>
       <c r="AM26" s="11"/>
@@ -5115,10 +5251,10 @@
         <v>12</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W27" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X27" s="2" t="s">
         <v>10</v>
@@ -5127,10 +5263,10 @@
         <v>10</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA27" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB27" s="2" t="s">
         <v>12</v>
@@ -5144,7 +5280,12 @@
       <c r="AE27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG27" s="11"/>
+      <c r="AF27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG27" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI27" s="11"/>
       <c r="AK27" s="11"/>
       <c r="AM27" s="11"/>
@@ -5210,25 +5351,25 @@
         <v>12</v>
       </c>
       <c r="T28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="V28" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="W28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Y28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA28" s="11" t="s">
         <v>12</v>
@@ -5245,16 +5386,21 @@
       <c r="AE28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG28" s="11"/>
+      <c r="AF28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG28" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI28" s="11"/>
       <c r="AK28" s="11"/>
       <c r="AM28" s="11"/>
       <c r="AO28" s="11"/>
       <c r="AQ28" s="11"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>12</v>
@@ -5311,10 +5457,10 @@
         <v>12</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V29" s="2" t="s">
         <v>12</v>
@@ -5335,10 +5481,10 @@
         <v>12</v>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AC29" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AD29" s="2" t="s">
         <v>12</v>
@@ -5346,7 +5492,12 @@
       <c r="AE29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AG29" s="11"/>
+      <c r="AF29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG29" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AI29" s="11"/>
       <c r="AK29" s="11"/>
       <c r="AM29" s="11"/>
@@ -5355,7 +5506,7 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>12</v>
@@ -5430,27 +5581,38 @@
         <v>12</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AB30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>12</v>
-      </c>
+      <c r="AF30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AM30" s="11"/>
+      <c r="AO30" s="11"/>
+      <c r="AQ30" s="11"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>12</v>
@@ -5525,306 +5687,431 @@
         <v>12</v>
       </c>
       <c r="Z31" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA31" s="11" t="s">
         <v>12</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AC31" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="AD31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="AE31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="X32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="T32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="V32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="B33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" t="s">
-        <v>12</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M33" t="s">
-        <v>12</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O33" t="s">
-        <v>12</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>12</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S33" t="s">
-        <v>12</v>
-      </c>
-      <c r="T33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U33" t="s">
-        <v>12</v>
-      </c>
-      <c r="V33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W33" t="s">
-        <v>12</v>
-      </c>
-      <c r="X33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC33" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:31" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="B34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" t="s">
+        <v>12</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>12</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S34" t="s">
+        <v>12</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U34" t="s">
+        <v>12</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W34" t="s">
+        <v>12</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC34" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" t="s">
-        <v>12</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M34" t="s">
-        <v>12</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O34" t="s">
-        <v>12</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>12</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S34" t="s">
-        <v>10</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U34" t="s">
-        <v>12</v>
-      </c>
-      <c r="V34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W34" t="s">
-        <v>12</v>
-      </c>
-      <c r="X34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE34" t="s">
+      <c r="B35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>12</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S35" t="s">
+        <v>10</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U35" t="s">
+        <v>12</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W35" t="s">
+        <v>12</v>
+      </c>
+      <c r="X35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG35" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5853,18 +6140,18 @@
     <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:AQ1048576">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576 M3:M1048576 O3:O1048576 Q3:Q1048576 S3:S1048576 U3:U1048576 W3:W1048576 Y3:Y1048576 AA3:AA1048576 AC3:AC1048576 AE3:AE1048576 AG3:AG1048576 AI3:AI1048576 AK3:AK1048576 AM3:AM1048576 AO3:AO1048576 AQ3:AQ1048576">
-    <cfRule type="expression" dxfId="6" priority="61">
+    <cfRule type="expression" dxfId="0" priority="61">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5913,7 +6200,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added functionality to "Fix Fields Metadata" Tool
</commit_message>
<xml_diff>
--- a/Data Standards+Metadata Checklist.xlsx
+++ b/Data Standards+Metadata Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHallock\Desktop\ArcGIS Scripts\Data Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58A9E6-B502-40EE-B5F6-9973FC262B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F242E2-AE40-461F-BAD4-FFC9D8938C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="103">
   <si>
     <t>Add Data Standards(Fields and MD)</t>
   </si>
@@ -259,9 +258,6 @@
     <t>Add Placeholders to MD values that should be filled</t>
   </si>
   <si>
-    <t>y (At end)</t>
-  </si>
-  <si>
     <t>Clean Print Messages</t>
   </si>
   <si>
@@ -271,9 +267,6 @@
     <t>AddDefaultsToNewField</t>
   </si>
   <si>
-    <t>Assign defualt value to a field</t>
-  </si>
-  <si>
     <t>*Edit values in table to match default</t>
   </si>
   <si>
@@ -326,6 +319,24 @@
   </si>
   <si>
     <t>Adds Placeholders when needed</t>
+  </si>
+  <si>
+    <t>DeleteDuplicateFieldsFromMD</t>
+  </si>
+  <si>
+    <t>AddFieldToMD</t>
+  </si>
+  <si>
+    <t>Assign default value to a field</t>
+  </si>
+  <si>
+    <t>RenameFieldMetadata</t>
+  </si>
+  <si>
+    <t>SynchronizeMetadata</t>
+  </si>
+  <si>
+    <t>Synchronize Metadata</t>
   </si>
 </sst>
 </file>
@@ -1095,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1150,7 @@
       </c>
       <c r="K1" s="27"/>
       <c r="L1" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M1" s="27"/>
       <c r="N1" s="21"/>
@@ -1192,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -1216,7 +1227,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -1244,7 +1255,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
@@ -1313,7 +1324,7 @@
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
@@ -1477,7 +1488,7 @@
     </row>
     <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
@@ -1518,7 +1529,7 @@
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
@@ -1618,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>12</v>
@@ -1700,13 +1711,13 @@
         <v>10</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>12</v>
@@ -1741,13 +1752,13 @@
         <v>10</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>12</v>
@@ -1782,13 +1793,13 @@
         <v>10</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>12</v>
@@ -1820,16 +1831,16 @@
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>12</v>
@@ -1864,7 +1875,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>12</v>
@@ -1905,7 +1916,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>12</v>
@@ -1946,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>12</v>
@@ -1984,7 +1995,7 @@
         <v>12</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>12</v>
@@ -2025,7 +2036,7 @@
         <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>12</v>
@@ -2066,7 +2077,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>12</v>
@@ -2256,7 +2267,7 @@
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>12</v>
@@ -2297,7 +2308,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>12</v>
@@ -2384,11 +2395,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D037D56-654E-4299-841C-27C58773C05D}">
-  <dimension ref="A1:AR35"/>
+  <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V17" sqref="V17"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2408,8 +2419,8 @@
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
     <col min="18" max="18" width="13.28515625" style="2" customWidth="1"/>
     <col min="19" max="19" width="13.28515625" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" style="2" customWidth="1"/>
@@ -2445,15 +2456,15 @@
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="27"/>
       <c r="F1" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G1" s="27"/>
       <c r="H1" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="26" t="s">
@@ -2469,48 +2480,56 @@
       </c>
       <c r="O1" s="27"/>
       <c r="P1" s="26" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="Q1" s="27"/>
       <c r="R1" s="26" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="S1" s="27"/>
       <c r="T1" s="26" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="U1" s="27"/>
       <c r="V1" s="26" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="W1" s="27"/>
       <c r="X1" s="26" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="Y1" s="27"/>
       <c r="Z1" s="26" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="AA1" s="27"/>
       <c r="AB1" s="26" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AC1" s="27"/>
       <c r="AD1" s="26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE1" s="27"/>
       <c r="AF1" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" s="27"/>
+      <c r="AJ1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM1" s="27"/>
+      <c r="AN1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="26"/>
       <c r="AO1" s="27"/>
       <c r="AP1" s="29"/>
       <c r="AQ1" s="29"/>
@@ -2692,13 +2711,13 @@
         <v>10</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="T3" s="2" t="s">
         <v>10</v>
@@ -2716,7 +2735,7 @@
         <v>10</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>10</v>
@@ -2734,7 +2753,7 @@
         <v>10</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>10</v>
@@ -2742,10 +2761,30 @@
       <c r="AG3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI3" s="11"/>
-      <c r="AK3" s="11"/>
-      <c r="AM3" s="11"/>
-      <c r="AO3" s="11"/>
+      <c r="AH3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ3" s="11"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
@@ -2756,102 +2795,122 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AO4" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM4" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO4" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ4" s="11"/>
     </row>
     <row r="5" spans="1:44" ht="30" x14ac:dyDescent="0.25">
@@ -2862,102 +2921,122 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG5" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AM5" s="11"/>
-      <c r="AO5" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO5" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ5" s="11"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
@@ -2968,102 +3047,122 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE6" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG6" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AM6" s="11"/>
-      <c r="AO6" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO6" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ6" s="11"/>
     </row>
     <row r="7" spans="1:44" ht="30" x14ac:dyDescent="0.25">
@@ -3074,102 +3173,122 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE7" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG7" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI7" s="11"/>
-      <c r="AK7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AO7" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO7" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ7" s="11"/>
     </row>
     <row r="8" spans="1:44" ht="30" x14ac:dyDescent="0.25">
@@ -3180,208 +3299,248 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG8" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI8" s="11"/>
-      <c r="AK8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AO8" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO8" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ8" s="11"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE9" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG9" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AO9" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO9" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ9" s="11"/>
     </row>
     <row r="10" spans="1:44" ht="30" x14ac:dyDescent="0.25">
@@ -3392,208 +3551,248 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE10" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AO10" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO10" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ10" s="11"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="W11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Z11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AB11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AC11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AD11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AE11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AF11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AM11" s="11"/>
-      <c r="AO11" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM11" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO11" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="AQ11" s="11"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
@@ -3696,10 +3895,30 @@
       <c r="AG12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI12" s="11"/>
-      <c r="AK12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AO12" s="11"/>
+      <c r="AH12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO12" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ12" s="11"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
@@ -3802,10 +4021,30 @@
       <c r="AG13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AO13" s="11"/>
+      <c r="AH13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO13" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ13" s="11"/>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
@@ -3908,10 +4147,30 @@
       <c r="AG14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AO14" s="11"/>
+      <c r="AH14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO14" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ14" s="11"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
@@ -4014,15 +4273,35 @@
       <c r="AG15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AO15" s="11"/>
+      <c r="AH15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO15" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ15" s="11"/>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -4120,15 +4399,35 @@
       <c r="AG16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AM16" s="11"/>
-      <c r="AO16" s="11"/>
+      <c r="AH16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO16" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ16" s="11"/>
     </row>
     <row r="17" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -4226,15 +4525,35 @@
       <c r="AG17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI17" s="11"/>
-      <c r="AK17" s="11"/>
-      <c r="AM17" s="11"/>
-      <c r="AO17" s="11"/>
+      <c r="AH17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO17" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ17" s="11"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -4332,15 +4651,35 @@
       <c r="AG18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AM18" s="11"/>
-      <c r="AO18" s="11"/>
+      <c r="AH18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO18" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ18" s="11"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>12</v>
@@ -4438,15 +4777,35 @@
       <c r="AG19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI19" s="11"/>
-      <c r="AK19" s="11"/>
-      <c r="AM19" s="11"/>
-      <c r="AO19" s="11"/>
+      <c r="AH19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO19" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ19" s="11"/>
     </row>
     <row r="20" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>12</v>
@@ -4470,7 +4829,7 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>12</v>
@@ -4544,10 +4903,30 @@
       <c r="AG20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI20" s="11"/>
-      <c r="AK20" s="11"/>
-      <c r="AM20" s="11"/>
-      <c r="AO20" s="11"/>
+      <c r="AH20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO20" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ20" s="11"/>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
@@ -4633,27 +5012,47 @@
         <v>10</v>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AC21" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE21" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI21" s="11"/>
-      <c r="AK21" s="11"/>
-      <c r="AM21" s="11"/>
-      <c r="AO21" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO21" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ21" s="11"/>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
@@ -4739,27 +5138,47 @@
         <v>10</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AC22" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE22" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AM22" s="11"/>
-      <c r="AO22" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO22" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ22" s="11"/>
     </row>
     <row r="23" spans="1:43" ht="45" x14ac:dyDescent="0.25">
@@ -4830,42 +5249,62 @@
         <v>10</v>
       </c>
       <c r="W23" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Y23" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Z23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="AA23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AB23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI23" s="11"/>
-      <c r="AK23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AO23" s="11"/>
+      <c r="AH23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO23" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ23" s="11"/>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
@@ -4933,45 +5372,65 @@
         <v>12</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W24" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Y24" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA24" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AC24" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AD24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE24" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI24" s="11"/>
-      <c r="AK24" s="11"/>
-      <c r="AM24" s="11"/>
-      <c r="AO24" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO24" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ24" s="11"/>
     </row>
     <row r="25" spans="1:43" ht="30" x14ac:dyDescent="0.25">
@@ -5039,45 +5498,65 @@
         <v>12</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W25" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Y25" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA25" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AC25" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE25" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI25" s="11"/>
-      <c r="AK25" s="11"/>
-      <c r="AM25" s="11"/>
-      <c r="AO25" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO25" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ25" s="11"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
@@ -5145,45 +5624,65 @@
         <v>12</v>
       </c>
       <c r="V26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB26" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="AC26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE26" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI26" s="11"/>
-      <c r="AK26" s="11"/>
-      <c r="AM26" s="11"/>
-      <c r="AO26" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO26" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ26" s="11"/>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -5257,16 +5756,16 @@
         <v>12</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Y27" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA27" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB27" s="2" t="s">
         <v>12</v>
@@ -5275,21 +5774,41 @@
         <v>12</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AE27" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF27" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AM27" s="11"/>
-      <c r="AO27" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="AH27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO27" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ27" s="11"/>
     </row>
     <row r="28" spans="1:43" ht="30" x14ac:dyDescent="0.25">
@@ -5357,26 +5876,26 @@
         <v>12</v>
       </c>
       <c r="V28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="X28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="X28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB28" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="AC28" s="11" t="s">
         <v>12</v>
       </c>
@@ -5387,20 +5906,40 @@
         <v>12</v>
       </c>
       <c r="AF28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AG28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI28" s="11"/>
-      <c r="AK28" s="11"/>
-      <c r="AM28" s="11"/>
-      <c r="AO28" s="11"/>
+      <c r="AH28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO28" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ28" s="11"/>
     </row>
     <row r="29" spans="1:43" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>12</v>
@@ -5457,10 +5996,10 @@
         <v>12</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V29" s="2" t="s">
         <v>12</v>
@@ -5475,10 +6014,10 @@
         <v>12</v>
       </c>
       <c r="Z29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA29" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AB29" s="2" t="s">
         <v>12</v>
@@ -5498,10 +6037,30 @@
       <c r="AG29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI29" s="11"/>
-      <c r="AK29" s="11"/>
-      <c r="AM29" s="11"/>
-      <c r="AO29" s="11"/>
+      <c r="AH29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO29" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ29" s="11"/>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
@@ -5593,21 +6152,41 @@
         <v>12</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AE30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AF30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI30" s="11"/>
-      <c r="AK30" s="11"/>
-      <c r="AM30" s="11"/>
-      <c r="AO30" s="11"/>
+      <c r="AL30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO30" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="AQ30" s="11"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
@@ -5693,21 +6272,45 @@
         <v>12</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AC31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI31" t="s">
         <v>18</v>
       </c>
-      <c r="AD31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG31" t="s">
+      <c r="AJ31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO31" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5794,7 +6397,7 @@
         <v>12</v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AC32" s="11" t="s">
         <v>12</v>
@@ -5811,8 +6414,32 @@
       <c r="AG32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>74</v>
       </c>
@@ -5895,13 +6522,13 @@
         <v>12</v>
       </c>
       <c r="AB33" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AC33" s="11" t="s">
         <v>12</v>
       </c>
       <c r="AD33" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AE33" t="s">
         <v>12</v>
@@ -5912,10 +6539,34 @@
       <c r="AG33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>12</v>
@@ -5962,13 +6613,13 @@
       <c r="P34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="Q34" s="11" t="s">
         <v>12</v>
       </c>
       <c r="R34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S34" t="s">
+      <c r="S34" s="11" t="s">
         <v>12</v>
       </c>
       <c r="T34" s="2" t="s">
@@ -5986,7 +6637,7 @@
       <c r="X34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Y34" s="11" t="s">
         <v>12</v>
       </c>
       <c r="Z34" s="2" t="s">
@@ -6008,120 +6659,288 @@
         <v>12</v>
       </c>
       <c r="AF34" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AG34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="AH34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" t="s">
+        <v>12</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U35" t="s">
+        <v>12</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W35" t="s">
+        <v>12</v>
+      </c>
+      <c r="X35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AO35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M35" t="s">
-        <v>12</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O35" t="s">
-        <v>12</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>12</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S35" t="s">
-        <v>10</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U35" t="s">
-        <v>12</v>
-      </c>
-      <c r="V35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W35" t="s">
-        <v>12</v>
-      </c>
-      <c r="X35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG35" t="s">
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U36" t="s">
+        <v>12</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W36" t="s">
+        <v>10</v>
+      </c>
+      <c r="X36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO36" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AP1:AQ1"/>
@@ -6138,6 +6957,11 @@
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:AQ1048576">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
@@ -6150,7 +6974,7 @@
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576 M3:M1048576 O3:O1048576 Q3:Q1048576 S3:S1048576 U3:U1048576 W3:W1048576 Y3:Y1048576 AA3:AA1048576 AC3:AC1048576 AE3:AE1048576 AG3:AG1048576 AI3:AI1048576 AK3:AK1048576 AM3:AM1048576 AO3:AO1048576 AQ3:AQ1048576">
+  <conditionalFormatting sqref="AQ3:AQ1048576 C3:C1048576 E3:E1048576 G3:G1048576 I3:I1048576 K3:K1048576 M3:M1048576 O3:O1048576 U3:U1048576 W3:W1048576 Y3:Y1048576 AA3:AA1048576 AC3:AC1048576 AE3:AE1048576 AG3:AG1048576 AI3:AI1048576 AK3:AK1048576 AM3:AM1048576 AO3:AO1048576 Q3:Q1048576 S3:S1048576">
     <cfRule type="expression" dxfId="0" priority="61">
       <formula>B3&lt;&gt;C3</formula>
     </cfRule>

</xml_diff>